<commit_message>
chore: changed workbook sheet and table naming; fix: fixed converters and services affected by workbook naming changes
</commit_message>
<xml_diff>
--- a/api/resources/excel/Commission/CommissionWorkbook.xlsx
+++ b/api/resources/excel/Commission/CommissionWorkbook.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="cw_summary" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="cw_signups" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="cw_purchases" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="commission_summary_sheet" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="signup_sheet" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="purchase_sheet" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +15,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="60">
   <si>
-    <t>commissions_summary_list</t>
+    <t>commission_summary_list</t>
   </si>
   <si>
     <t>headers</t>
@@ -105,7 +105,7 @@
     <t>total_commission</t>
   </si>
   <si>
-    <t>signup_commissions_table</t>
+    <t>signup_commission_table</t>
   </si>
   <si>
     <t>contact_id</t>
@@ -174,7 +174,7 @@
     <t>logolink</t>
   </si>
   <si>
-    <t>purchase_commissions_table</t>
+    <t>purchase_commission_table</t>
   </si>
   <si>
     <t>purchase_id</t>

</xml_diff>

<commit_message>
chore: Renamed purchase and signup sheets
</commit_message>
<xml_diff>
--- a/api/resources/excel/Commission/CommissionWorkbook.xlsx
+++ b/api/resources/excel/Commission/CommissionWorkbook.xlsx
@@ -105,7 +105,7 @@
     <t>total_commission</t>
   </si>
   <si>
-    <t>signup_commission_table</t>
+    <t>signup_table</t>
   </si>
   <si>
     <t>contact_id</t>
@@ -174,7 +174,7 @@
     <t>logolink</t>
   </si>
   <si>
-    <t>purchase_commission_table</t>
+    <t>purchase_table</t>
   </si>
   <si>
     <t>purchase_id</t>

</xml_diff>